<commit_message>
AFDP-2260: Remove 'Intake' queue from next possible queues in 'Suspend' queue
</commit_message>
<xml_diff>
--- a/acm/rules/drools-next-possible-queues-rules-foia.xlsx
+++ b/acm/rules/drools-next-possible-queues-rules-foia.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\Documents\foia-extension\src\main\resources\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dame.gjorgjievski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16388" windowHeight="8190" tabRatio="995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -988,23 +988,23 @@
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.73046875"/>
-    <col min="2" max="2" width="26.3984375"/>
-    <col min="3" max="3" width="103.6640625"/>
-    <col min="4" max="5" width="71.1328125"/>
-    <col min="6" max="6" width="35.73046875"/>
-    <col min="7" max="7" width="36.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.59765625"/>
-    <col min="9" max="1025" width="8.73046875"/>
+    <col min="1" max="1" width="14.75"/>
+    <col min="2" max="2" width="26.375"/>
+    <col min="3" max="3" width="103.625"/>
+    <col min="4" max="5" width="71.125"/>
+    <col min="6" max="6" width="35.75"/>
+    <col min="7" max="7" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.625"/>
+    <col min="9" max="1025" width="8.75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1014,7 +1014,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1025,7 +1025,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1036,7 +1036,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1047,7 +1047,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1058,7 +1058,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
@@ -1081,7 +1081,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
         <v>2</v>
       </c>
@@ -1093,7 +1093,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
         <v>2</v>
       </c>
@@ -1105,7 +1105,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1117,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
@@ -1129,7 +1129,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" s="6" t="s">
         <v>2</v>
       </c>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:8" ht="213.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" ht="225" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="9"/>
       <c r="C14" s="10" t="s">
         <v>15</v>
@@ -1165,12 +1165,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1179,7 +1179,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C17" s="4" t="s">
         <v>18</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
         <v>20</v>
       </c>
@@ -1205,7 +1205,7 @@
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" s="13" t="s">
         <v>21</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="114" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>24</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="19"/>
       <c r="B21" s="19" t="s">
         <v>29</v>
@@ -1264,7 +1264,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="19"/>
       <c r="B22" s="19" t="s">
         <v>32</v>
@@ -1283,7 +1283,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="19" t="s">
         <v>35</v>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="19" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F23" s="21" t="s">
         <v>38</v>
@@ -1302,7 +1302,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="19" t="s">
         <v>37</v>
@@ -1321,7 +1321,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="19" t="s">
         <v>40</v>
@@ -1342,7 +1342,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="19" t="s">
         <v>44</v>
@@ -1363,7 +1363,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="19" t="s">
         <v>47</v>
@@ -1384,7 +1384,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="19" t="s">
         <v>50</v>
@@ -1405,7 +1405,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="19" t="s">
         <v>53</v>
@@ -1426,7 +1426,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="19" t="s">
         <v>55</v>
@@ -1447,7 +1447,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="19" t="s">
         <v>58</v>
@@ -1468,7 +1468,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="19" t="s">
         <v>61</v>
@@ -1504,9 +1504,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875"/>
+    <col min="1" max="1025" width="8.75"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1523,9 +1523,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.73046875"/>
+    <col min="1" max="1025" width="8.75"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
AFDP-2327 Added 'Fulfill' to the list of possible next queues to all rules that have 'Fulfill' queue as a default return queue.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-next-possible-queues-rules-foia.xlsx
+++ b/acm/rules/drools-next-possible-queues-rules-foia.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dame.gjorgjievski\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazo.lazarev\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="71">
   <si>
     <t>RuleSet</t>
   </si>
@@ -189,27 +189,18 @@
     <t>!litigationFlag &amp;&amp; !"Appeal".equals(requestSubType) &amp;&amp; feeWaiverFlag</t>
   </si>
   <si>
-    <t>Release,Hold</t>
-  </si>
-  <si>
     <t>Approve to GC</t>
   </si>
   <si>
     <t>litigationFlag || "Appeal".equals(requestSubType)</t>
   </si>
   <si>
-    <t>General Counsel,Hold</t>
-  </si>
-  <si>
     <t>Approve to Billing</t>
   </si>
   <si>
     <t>!litigationFlag &amp;&amp; !"Appeal".equals(requestSubType) &amp;&amp; !feeWaiverFlag</t>
   </si>
   <si>
-    <t>Billing,Hold</t>
-  </si>
-  <si>
     <t>General Counsel to Billing</t>
   </si>
   <si>
@@ -265,6 +256,21 @@
   </si>
   <si>
     <t>$model.setDefaultReturnQueue($param);</t>
+  </si>
+  <si>
+    <t>Release,Hold,Fulfill</t>
+  </si>
+  <si>
+    <t>General Counsel,Hold,Fulfill</t>
+  </si>
+  <si>
+    <t>Billing,Hold,Fulfill</t>
+  </si>
+  <si>
+    <t>Hold,Fulfill</t>
+  </si>
+  <si>
+    <t>Release,Fulfill</t>
   </si>
 </sst>
 </file>
@@ -988,23 +994,23 @@
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="D19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.75"/>
-    <col min="2" max="2" width="26.375"/>
-    <col min="3" max="3" width="103.625"/>
-    <col min="4" max="5" width="71.125"/>
-    <col min="6" max="6" width="35.75"/>
-    <col min="7" max="7" width="36.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.625"/>
-    <col min="9" max="1025" width="8.75"/>
+    <col min="1" max="1" width="14.73046875"/>
+    <col min="2" max="2" width="26.3984375"/>
+    <col min="3" max="3" width="103.59765625"/>
+    <col min="4" max="5" width="71.1328125"/>
+    <col min="6" max="6" width="35.73046875"/>
+    <col min="7" max="7" width="36.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.59765625"/>
+    <col min="9" max="1025" width="8.73046875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1014,7 +1020,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1025,7 +1031,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1036,7 +1042,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1047,7 +1053,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C5" s="6" t="s">
         <v>2</v>
       </c>
@@ -1058,7 +1064,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
@@ -1069,7 +1075,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C7" s="6" t="s">
         <v>2</v>
       </c>
@@ -1081,7 +1087,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C8" s="6" t="s">
         <v>2</v>
       </c>
@@ -1093,7 +1099,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C9" s="6" t="s">
         <v>2</v>
       </c>
@@ -1105,7 +1111,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C10" s="6" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1123,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C11" s="6" t="s">
         <v>2</v>
       </c>
@@ -1129,7 +1135,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C12" s="6" t="s">
         <v>2</v>
       </c>
@@ -1138,7 +1144,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:8" ht="225" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="213.75" x14ac:dyDescent="0.45">
       <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1147,7 +1153,7 @@
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B14" s="9"/>
       <c r="C14" s="10" t="s">
         <v>15</v>
@@ -1165,12 +1171,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1179,7 +1185,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C17" s="4" t="s">
         <v>18</v>
       </c>
@@ -1196,7 +1202,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C18" s="4" t="s">
         <v>20</v>
       </c>
@@ -1205,7 +1211,7 @@
       <c r="F18" s="12"/>
       <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C19" s="13" t="s">
         <v>21</v>
       </c>
@@ -1216,13 +1222,13 @@
         <v>23</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="114" x14ac:dyDescent="0.45">
       <c r="A20" s="15" t="s">
         <v>24</v>
       </c>
@@ -1239,13 +1245,13 @@
         <v>28</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="19"/>
       <c r="B21" s="19" t="s">
         <v>29</v>
@@ -1261,10 +1267,10 @@
         <v>38</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="19"/>
       <c r="B22" s="19" t="s">
         <v>32</v>
@@ -1280,10 +1286,10 @@
         <v>38</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="19"/>
       <c r="B23" s="19" t="s">
         <v>35</v>
@@ -1299,10 +1305,10 @@
         <v>38</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="19"/>
       <c r="B24" s="19" t="s">
         <v>37</v>
@@ -1318,10 +1324,10 @@
         <v>41</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="19"/>
       <c r="B25" s="19" t="s">
         <v>40</v>
@@ -1333,158 +1339,158 @@
         <v>42</v>
       </c>
       <c r="E25" s="19" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="19"/>
       <c r="B26" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="20" t="s">
         <v>41</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="F26" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="19"/>
       <c r="B27" s="19" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" s="20" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E27" s="19" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="19"/>
       <c r="B28" s="19" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="19"/>
       <c r="B29" s="19" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C29" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="20" t="s">
-        <v>54</v>
-      </c>
       <c r="E29" s="19" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="19"/>
       <c r="B30" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>33</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="19"/>
       <c r="B31" s="19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C31" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D31" s="20" t="s">
-        <v>59</v>
-      </c>
       <c r="E31" s="19" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="19"/>
       <c r="B32" s="19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1504,9 +1510,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.75"/>
+    <col min="1" max="1025" width="8.73046875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1523,9 +1529,9 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1025" width="8.75"/>
+    <col min="1" max="1025" width="8.73046875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Intake queue removed from possible queues for Hold queue.
</commit_message>
<xml_diff>
--- a/acm/rules/drools-next-possible-queues-rules-foia.xlsx
+++ b/acm/rules/drools-next-possible-queues-rules-foia.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dame.gjorgjievski\.arkcase\acm\rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dragan.simonovski\.arkcase\acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
   <si>
     <t>RuleSet</t>
   </si>
@@ -160,9 +160,6 @@
   </si>
   <si>
     <t>Hold</t>
-  </si>
-  <si>
-    <t>Fulfill,Intake</t>
   </si>
   <si>
     <t>Suspend Next Queues</t>
@@ -988,20 +985,20 @@
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.75"/>
-    <col min="2" max="2" width="26.375"/>
-    <col min="3" max="3" width="103.625"/>
-    <col min="4" max="5" width="71.125"/>
-    <col min="6" max="6" width="35.75"/>
-    <col min="7" max="7" width="36.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.625"/>
-    <col min="9" max="1025" width="8.75"/>
+    <col min="1" max="1" width="14.7109375"/>
+    <col min="2" max="2" width="26.42578125"/>
+    <col min="3" max="3" width="103.5703125"/>
+    <col min="4" max="5" width="71.140625"/>
+    <col min="6" max="6" width="35.7109375"/>
+    <col min="7" max="7" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.5703125"/>
+    <col min="9" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1216,13 +1213,13 @@
         <v>23</v>
       </c>
       <c r="F19" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G19" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G19" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
         <v>24</v>
       </c>
@@ -1239,10 +1236,10 @@
         <v>28</v>
       </c>
       <c r="F20" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1258,10 +1255,10 @@
         <v>31</v>
       </c>
       <c r="F21" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1274,168 +1271,168 @@
       </c>
       <c r="D22" s="20"/>
       <c r="E22" s="19" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="19"/>
       <c r="B23" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>35</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>36</v>
       </c>
       <c r="D23" s="20"/>
       <c r="E23" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="19"/>
       <c r="B24" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>37</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>38</v>
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="19"/>
       <c r="B25" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="D25" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="E25" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="19" t="s">
-        <v>43</v>
-      </c>
       <c r="F25" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G25" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="19"/>
       <c r="B26" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="20" t="s">
+      <c r="E26" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="E26" s="19" t="s">
-        <v>46</v>
-      </c>
       <c r="F26" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="19"/>
       <c r="B27" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="20" t="s">
+      <c r="E27" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>49</v>
-      </c>
       <c r="F27" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G27" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="19"/>
       <c r="B28" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="20" t="s">
+      <c r="D28" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="20" t="s">
-        <v>52</v>
-      </c>
       <c r="E28" s="19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G28" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="19"/>
       <c r="B29" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>54</v>
-      </c>
       <c r="E29" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G29" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="19"/>
       <c r="B30" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="D30" s="20" t="s">
         <v>56</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>57</v>
       </c>
       <c r="E30" s="19" t="s">
         <v>33</v>
@@ -1444,47 +1441,47 @@
         <v>33</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="19"/>
       <c r="B31" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="C31" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="D31" s="20" t="s">
+      <c r="E31" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="19" t="s">
-        <v>60</v>
-      </c>
       <c r="F31" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G31" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="19"/>
       <c r="B32" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="20" t="s">
         <v>61</v>
-      </c>
-      <c r="C32" s="20" t="s">
-        <v>62</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G32" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1506,7 +1503,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.75"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1525,7 +1522,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="8.75"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
for billing queue Fulfill is removed from nextpossible queues. eventType added for Request Updated
</commit_message>
<xml_diff>
--- a/acm/rules/drools-next-possible-queues-rules-foia.xlsx
+++ b/acm/rules/drools-next-possible-queues-rules-foia.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
   <si>
     <t>RuleSet</t>
   </si>
@@ -262,12 +262,6 @@
   </si>
   <si>
     <t>Billing,Hold,Fulfill</t>
-  </si>
-  <si>
-    <t>Hold,Fulfill</t>
-  </si>
-  <si>
-    <t>Release,Fulfill</t>
   </si>
 </sst>
 </file>
@@ -991,8 +985,8 @@
   </sheetPr>
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,7 +1435,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>68</v>
+        <v>33</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>33</v>
@@ -1462,7 +1456,7 @@
         <v>55</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
Fulfill return as next queue for Billing queue
</commit_message>
<xml_diff>
--- a/acm/rules/drools-next-possible-queues-rules-foia.xlsx
+++ b/acm/rules/drools-next-possible-queues-rules-foia.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
   <si>
     <t>RuleSet</t>
   </si>
@@ -262,6 +262,12 @@
   </si>
   <si>
     <t>Billing,Hold,Fulfill</t>
+  </si>
+  <si>
+    <t>Hold,Fulfill</t>
+  </si>
+  <si>
+    <t>Release,Fulfill</t>
   </si>
 </sst>
 </file>
@@ -986,7 +992,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1435,7 +1441,7 @@
         <v>53</v>
       </c>
       <c r="E30" s="19" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="F30" s="21" t="s">
         <v>33</v>
@@ -1456,7 +1462,7 @@
         <v>55</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>56</v>

</xml_diff>